<commit_message>
Testing all suitcases and changing xpaths
</commit_message>
<xml_diff>
--- a/test_info/data/HU1-001/CP-001/objects.xlsx
+++ b/test_info/data/HU1-001/CP-001/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan_piedrahita\Documents\jp\bvc\tests\A2censoTest\test_info\data\HU1-001\CP-001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF973A61-9068-4BE5-A07B-2DE84F1A7668}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10698F8-668B-4C55-991C-44DD2230E355}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{58DB2863-25CE-48F2-AA27-D6192448486C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{58DB2863-25CE-48F2-AA27-D6192448486C}"/>
   </bookViews>
   <sheets>
     <sheet name="menu" sheetId="2" r:id="rId1"/>
@@ -40,9 +40,6 @@
     <t>footer</t>
   </si>
   <si>
-    <t>/html/body/div[1]/div/div/section/section[7]/div/div[1]/div[1]</t>
-  </si>
-  <si>
     <t>xpath</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>link</t>
   </si>
   <si>
-    <t>/html/body/div[1]/div/div/div[1]/div[1]/div/nav/div[3]/button</t>
-  </si>
-  <si>
     <t>menu</t>
   </si>
   <si>
@@ -112,9 +106,6 @@
     <t>Vitrina</t>
   </si>
   <si>
-    <t>/html/body/div[1]/div/div/div[1]/div[1]/div/nav/div[1]/img</t>
-  </si>
-  <si>
     <t>navbar</t>
   </si>
   <si>
@@ -122,6 +113,15 @@
   </si>
   <si>
     <t>/html/body/div[1]/div/div/div[5]/div</t>
+  </si>
+  <si>
+    <t>//*[@id="root"]/div/div/div[1]/div[1]/div/nav/div[1]/a/img</t>
+  </si>
+  <si>
+    <t>//*[@id="root"]/div/div/div[1]/div[1]/div/nav/div[3]/button</t>
+  </si>
+  <si>
+    <t>//*[@id="footer"]</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -511,86 +511,86 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -605,7 +605,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -629,72 +629,72 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -702,27 +702,27 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating xpaths and adding wait for buttos
</commit_message>
<xml_diff>
--- a/test_info/data/HU1-001/CP-001/objects.xlsx
+++ b/test_info/data/HU1-001/CP-001/objects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan_piedrahita\Documents\jp\bvc\tests\A2censoTest\test_info\data\HU1-001\CP-001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10698F8-668B-4C55-991C-44DD2230E355}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED2BAA8-09DD-449E-9B8B-D22B633D4639}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{58DB2863-25CE-48F2-AA27-D6192448486C}"/>
   </bookViews>
@@ -112,9 +112,6 @@
     <t>visible</t>
   </si>
   <si>
-    <t>/html/body/div[1]/div/div/div[5]/div</t>
-  </si>
-  <si>
     <t>//*[@id="root"]/div/div/div[1]/div[1]/div/nav/div[1]/a/img</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>//*[@id="footer"]</t>
+  </si>
+  <si>
+    <t>//*[@id="root"]/div/div/div[4]/div/div[1]/img</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>27</v>
@@ -587,7 +587,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>27</v>
@@ -605,7 +605,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +649,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>27</v>
@@ -705,7 +705,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>27</v>
@@ -719,7 +719,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>27</v>

</xml_diff>